<commit_message>
Outputs from updated input files.
</commit_message>
<xml_diff>
--- a/results/alldb_top_count_receptor.xlsx
+++ b/results/alldb_top_count_receptor.xlsx
@@ -392,26 +392,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EGF_EGFR</t>
+          <t>IL6_IL6R</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EGF</t>
+          <t>IL6</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>EGFR</t>
+          <t>IL6R</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CCIDB_Human_new.xlsx; CellChatDB.humanv2-2023-Jin-LR-pairs_new.xlsx; Human-2010-Kirouac-LR-pairs_new.xlsx; Human-2014-Qiao-LR-pairs.xlsx; Human-2015-Choi-LR-pairs.txt; Human-2015-Ramilowski-LR-pairs.xlsx; Human-2017-Pavlicev-LR-pairs.xlsx; Human-2019-Wang-LR-pairs.csv; Human-2019-Ximerakis-BaderLab-2017_new.xlsx; Human-2020-Hou-LR-pairs.xlsx; Human-2020-Shao-LR-pairs.txt; ICELLNETdb_v2_new.xlsx; interaction_input_Vento_Cellphonedbv5_new.csv; LRdb_122019_SingleCellSignalIR.xlsx; NicheNet-LR-pairs.csv; OmniPathPPIs_new.tsv</t>
+          <t>CCIDB_Human_new.xlsx; Human-2014-Qiao-LR-pairs.xlsx; Human-2015-Choi-LR-pairs.txt; Human-2015-Ramilowski-LR-pairs.xlsx; Human-2017-Pavlicev-LR-pairs.xlsx; Human-2019-Wang-LR-pairs.csv; Human-2019-Ximerakis-BaderLab-2017_new.xlsx; Human-2020-Hou-LR-pairs.xlsx; Human-2020-Shao-LR-pairs.txt; ICELLNETdb_v2_new.xlsx; LRdb_122019_SingleCellSignalIR.xlsx; NicheNet-LR-pairs.csv; OmniPathPPIs_new.tsv</t>
         </is>
       </c>
       <c r="E2">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
New results with updated ximerakis.
</commit_message>
<xml_diff>
--- a/results/alldb_top_count_receptor.xlsx
+++ b/results/alldb_top_count_receptor.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,41 +383,6 @@
           <t>count</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>"receptor(s)"</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>IL6_IL6R</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>IL6</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>IL6R</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CCIDB_Human_new.xlsx; Human-2014-Qiao-LR-pairs.xlsx; Human-2015-Choi-LR-pairs.txt; Human-2015-Ramilowski-LR-pairs.xlsx; Human-2017-Pavlicev-LR-pairs.xlsx; Human-2019-Wang-LR-pairs.csv; Human-2019-Ximerakis-BaderLab-2017_new.xlsx; Human-2020-Hou-LR-pairs.xlsx; Human-2020-Shao-LR-pairs.txt; ICELLNETdb_v2_new.xlsx; LRdb_122019_SingleCellSignalIR.xlsx; NicheNet-LR-pairs.csv; OmniPathPPIs_new.tsv</t>
-        </is>
-      </c>
-      <c r="E2">
-        <v>41</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>receptor(s)</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>